<commit_message>
small change to water automation
</commit_message>
<xml_diff>
--- a/Automation/Automations.xlsx
+++ b/Automation/Automations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matia\Desktop\Iot-Lab\Iot-Lab\Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iot_lab\Iot-Lab\Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C40EEE-F9EA-4BC9-A839-2957530F5244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7661D60-689D-43E5-B5DF-2BE0858EDE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC728893-7F4C-48FD-900F-C952A33424A5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CC728893-7F4C-48FD-900F-C952A33424A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>Productie Hoog</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://powermoves.blog/guides/home-automation-ideas/ </t>
+  </si>
+  <si>
+    <t>Vergelijking maken met humidity buiten om te weten of het wel nuttig is om ramen open te zetten</t>
   </si>
 </sst>
 </file>
@@ -563,21 +566,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A66BAD3-99C6-4FD5-990C-59257A931263}">
   <dimension ref="B2:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="75.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
@@ -585,7 +588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>22</v>
       </c>
@@ -599,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="L4" s="1" t="s">
         <v>9</v>
       </c>
@@ -607,7 +610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>24</v>
       </c>
@@ -621,7 +624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="L6" s="1" t="s">
         <v>13</v>
       </c>
@@ -629,7 +632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>26</v>
       </c>
@@ -643,7 +646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="L8" s="1" t="s">
         <v>16</v>
       </c>
@@ -651,7 +654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C9" s="4" t="s">
         <v>28</v>
       </c>
@@ -665,12 +668,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="L10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>31</v>
       </c>
@@ -684,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="L12" s="1" t="s">
         <v>21</v>
       </c>
@@ -692,7 +695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>33</v>
       </c>
@@ -700,7 +703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -711,7 +714,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -722,12 +725,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="L17" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>0</v>
       </c>
@@ -738,12 +741,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
@@ -751,7 +757,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -759,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>39</v>
       </c>
@@ -770,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>40</v>
       </c>
@@ -781,7 +787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>43</v>
       </c>
@@ -808,7 +814,7 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
small changes to automation
</commit_message>
<xml_diff>
--- a/Automation/Automations.xlsx
+++ b/Automation/Automations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iot_lab\Iot-Lab\Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7661D60-689D-43E5-B5DF-2BE0858EDE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF54544-2687-4CC3-BBA2-F893A9416DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CC728893-7F4C-48FD-900F-C952A33424A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Productie Hoog</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>Vergelijking maken met humidity buiten om te weten of het wel nuttig is om ramen open te zetten</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=VgV_ExVeSfE&amp;ab_channel=SmartHomeJunkie</t>
+  </si>
+  <si>
+    <t>automatisch tijden waarop het lokaal bezet is uitlezen ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kan ook op het dashboard gezet worden</t>
   </si>
 </sst>
 </file>
@@ -566,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A66BAD3-99C6-4FD5-990C-59257A931263}">
   <dimension ref="B2:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -764,6 +773,9 @@
       <c r="D22" t="s">
         <v>1</v>
       </c>
+      <c r="E22" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
@@ -782,6 +794,12 @@
       </c>
       <c r="D26" t="s">
         <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26" t="s">
+        <v>48</v>
       </c>
       <c r="R26" t="s">
         <v>2</v>
@@ -800,9 +818,10 @@
   <hyperlinks>
     <hyperlink ref="L17" r:id="rId1" xr:uid="{FE793C72-8A35-4F0A-B56A-A85845502858}"/>
     <hyperlink ref="L18" r:id="rId2" xr:uid="{5FC9022E-F868-4DA8-BE51-109F1F61C6D6}"/>
+    <hyperlink ref="E22" r:id="rId3" xr:uid="{CCB86141-D076-4975-8151-D35550CCD9F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>